<commit_message>
changed from excel to mongodb
</commit_message>
<xml_diff>
--- a/peertopeer.xlsx
+++ b/peertopeer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TUP\ECOPULSE\backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB841FC9-63A4-42EF-A49C-0509F3B09733}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB14F934-0E7F-44F2-BC55-3955FD93C282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="20986" windowHeight="13333" xr2:uid="{7F1E3285-8544-4C42-9346-025A8A19DF7D}"/>
   </bookViews>
@@ -538,7 +538,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4681308E-5448-455D-8EE6-4766F7EAF94B}">
   <dimension ref="A1:AS1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AH2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="AR2" sqref="AR2:AS20"/>
     </sheetView>
   </sheetViews>

</xml_diff>